<commit_message>
minor code updates and added craypat test
</commit_message>
<xml_diff>
--- a/perf_data.xlsx
+++ b/perf_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>N</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>% peak</t>
+  </si>
+  <si>
+    <t>L1 miss</t>
+  </si>
+  <si>
+    <t>L2 miss</t>
+  </si>
+  <si>
+    <t>L3 miss</t>
+  </si>
+  <si>
+    <t>opIRAM</t>
+  </si>
+  <si>
+    <t>opIL2</t>
+  </si>
+  <si>
+    <t>opIL3</t>
   </si>
 </sst>
 </file>
@@ -533,10 +551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -548,10 +566,12 @@
     <col min="9" max="9" width="6.28515625"/>
     <col min="10" max="10" width="8.5703125" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="1024" width="11.85546875"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="1024" width="11.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +605,26 @@
       <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>64</v>
       </c>
@@ -613,22 +651,43 @@
         <v>7644400000.0000019</v>
       </c>
       <c r="H2" s="1">
-        <v>16094417384</v>
+        <v>5340121898</v>
       </c>
       <c r="I2" s="2">
         <f>G2/H2</f>
-        <v>0.47497214826797995</v>
+        <v>1.4315029031196849</v>
       </c>
       <c r="J2" s="2">
-        <f>G2/(MIN(E2:F2)+ABS(F2-E2))</f>
-        <v>1.7426708612592896</v>
+        <f>2*G2/(MIN(E2:F2)+ABS(F2-E2))</f>
+        <v>3.4853417225185792</v>
       </c>
       <c r="K2" s="3">
         <f>I2/J2</f>
-        <v>0.27255413447652149</v>
+        <v>0.41072096141128211</v>
+      </c>
+      <c r="L2">
+        <v>446656891</v>
+      </c>
+      <c r="M2">
+        <v>19796</v>
+      </c>
+      <c r="N2">
+        <v>1204</v>
+      </c>
+      <c r="O2">
+        <f>$G$2/(L2*64)</f>
+        <v>0.26741723324268613</v>
+      </c>
+      <c r="P2">
+        <f>$G$2/(M2*64)</f>
+        <v>6033.7315619317051</v>
+      </c>
+      <c r="Q2">
+        <f>$G$2/(N2*64)</f>
+        <v>99205.77242524919</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>32</v>
       </c>
@@ -655,19 +714,40 @@
         <v>177880000</v>
       </c>
       <c r="H3" s="1">
-        <v>375677456</v>
+        <v>163971017</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3" si="8">G3/H3</f>
-        <v>0.47349128130808038</v>
+        <v>1.0848258628535554</v>
       </c>
       <c r="J3" s="2">
-        <f>G3/(MIN(E3:F3)+ABS(F3-E3))</f>
-        <v>1.7463184763400745</v>
+        <f>2*G3/(MIN(E3:F3)+ABS(F3-E3))</f>
+        <v>3.4926369526801491</v>
       </c>
       <c r="K3" s="3">
         <f>I3/J3</f>
-        <v>0.27113684458084703</v>
+        <v>0.31060367211115125</v>
+      </c>
+      <c r="L3">
+        <v>891600</v>
+      </c>
+      <c r="M3">
+        <v>10696</v>
+      </c>
+      <c r="N3">
+        <v>1147</v>
+      </c>
+      <c r="O3">
+        <f>$G$2/(L3*64)</f>
+        <v>133.96562359802604</v>
+      </c>
+      <c r="P3">
+        <f>$G$2/(M3*64)</f>
+        <v>11167.141922213914</v>
+      </c>
+      <c r="Q3">
+        <f>$G$2/(N3*64)</f>
+        <v>104135.7890148213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>